<commit_message>
jn: version luego de revision pa
</commit_message>
<xml_diff>
--- a/03_Entregable 1/Cronograma.xlsx
+++ b/03_Entregable 1/Cronograma.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF59F3B8-5698-4CBC-9EDD-A28D6A7C38EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A entregar" sheetId="1" r:id="rId1"/>
     <sheet name="Interno" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Producto</t>
   </si>
@@ -104,11 +103,17 @@
   <si>
     <t>Presentación del equipo consultor y socialización de estrategia de diagnóstico.</t>
   </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Semana</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +168,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +211,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -247,38 +264,390 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
       </left>
       <right style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
       </right>
       <top style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
       </left>
       <right style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
       </left>
       <right style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="7" tint="0.59999389629810485"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -290,7 +659,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -328,9 +697,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -340,19 +706,130 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Estilo 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Estilo 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Estilo 1" xfId="1"/>
+    <cellStyle name="Estilo 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -369,9 +846,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,9 +886,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +923,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,7 +958,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -654,833 +1131,880 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BL62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
-    <col min="3" max="24" width="3.7109375" style="1"/>
-    <col min="25" max="65" width="3.7109375" style="5"/>
-    <col min="66" max="16384" width="3.7109375" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="23" width="3.7109375" style="24"/>
+    <col min="24" max="64" width="3.7109375" style="25"/>
+    <col min="65" max="16384" width="3.7109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="71">
+        <v>1</v>
+      </c>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72">
         <v>2</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="14">
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72">
+        <v>3</v>
+      </c>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72">
+        <v>5</v>
+      </c>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="73"/>
+    </row>
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="68">
         <v>1</v>
       </c>
-      <c r="D2" s="14">
+      <c r="E2" s="69">
         <v>2</v>
       </c>
-      <c r="E2" s="14">
+      <c r="F2" s="69">
         <v>3</v>
       </c>
-      <c r="F2" s="14">
+      <c r="G2" s="69">
         <v>4</v>
       </c>
-      <c r="G2" s="14">
+      <c r="H2" s="69">
         <v>5</v>
       </c>
-      <c r="H2" s="14">
+      <c r="I2" s="69">
         <v>6</v>
       </c>
-      <c r="I2" s="14">
+      <c r="J2" s="69">
         <v>7</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="69">
         <v>8</v>
       </c>
-      <c r="K2" s="14">
+      <c r="L2" s="69">
         <v>9</v>
       </c>
-      <c r="L2" s="14">
+      <c r="M2" s="69">
         <v>10</v>
       </c>
-      <c r="M2" s="14">
+      <c r="N2" s="69">
         <v>11</v>
       </c>
-      <c r="N2" s="14">
+      <c r="O2" s="69">
         <v>12</v>
       </c>
-      <c r="O2" s="14">
+      <c r="P2" s="69">
         <v>13</v>
       </c>
-      <c r="P2" s="14">
+      <c r="Q2" s="69">
         <v>14</v>
       </c>
-      <c r="Q2" s="14">
+      <c r="R2" s="69">
         <v>15</v>
       </c>
-      <c r="R2" s="14">
+      <c r="S2" s="69">
         <v>16</v>
       </c>
-      <c r="S2" s="14">
+      <c r="T2" s="69">
         <v>17</v>
       </c>
-      <c r="T2" s="14">
+      <c r="U2" s="69">
         <v>18</v>
       </c>
-      <c r="U2" s="14">
+      <c r="V2" s="69">
         <v>19</v>
       </c>
-      <c r="V2" s="14">
+      <c r="W2" s="70">
         <v>20</v>
       </c>
-      <c r="W2" s="14">
+    </row>
+    <row r="3" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="43"/>
+    </row>
+    <row r="4" spans="1:23" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="42"/>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="37"/>
+    </row>
+    <row r="6" spans="1:23" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="43"/>
+    </row>
+    <row r="7" spans="1:23" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="39"/>
+      <c r="B7" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="41"/>
+    </row>
+    <row r="8" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="41"/>
+    </row>
+    <row r="9" spans="1:23" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="42"/>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="54"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="37"/>
+    </row>
+    <row r="11" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="43"/>
+    </row>
+    <row r="12" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="41"/>
+    </row>
+    <row r="13" spans="1:23" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="60"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="42"/>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="54"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="37"/>
+    </row>
+    <row r="15" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="63"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="43"/>
+    </row>
+    <row r="16" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
+      <c r="B16" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="49"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="41"/>
+    </row>
+    <row r="17" spans="1:23" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="52"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="42"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="54"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="37"/>
+    </row>
+    <row r="19" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="56"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="47"/>
+      <c r="W19" s="43"/>
+    </row>
+    <row r="20" spans="1:23" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-    </row>
-    <row r="4" spans="1:24" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-    </row>
-    <row r="6" spans="1:24" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-    </row>
-    <row r="7" spans="1:24" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-    </row>
-    <row r="8" spans="1:24" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-    </row>
-    <row r="9" spans="1:24" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-    </row>
-    <row r="11" spans="1:24" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-    </row>
-    <row r="12" spans="1:24" ht="57" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-    </row>
-    <row r="13" spans="1:24" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-    </row>
-    <row r="15" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-    </row>
-    <row r="16" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-    </row>
-    <row r="17" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-    </row>
-    <row r="19" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="8"/>
-    </row>
-    <row r="20" spans="1:24" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="7"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="12" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="48"/>
+    </row>
+    <row r="21" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="15"/>
-    </row>
-    <row r="22" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-    </row>
-    <row r="23" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-    </row>
-    <row r="24" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-    </row>
-    <row r="25" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-    </row>
-    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-    </row>
-    <row r="27" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-    </row>
-    <row r="28" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-    </row>
-    <row r="29" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-    </row>
-    <row r="30" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-    </row>
-    <row r="31" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-    </row>
-    <row r="32" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-    </row>
-    <row r="33" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-    </row>
-    <row r="34" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-    </row>
-    <row r="35" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-    </row>
-    <row r="36" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-    </row>
-    <row r="37" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-    </row>
-    <row r="38" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-    </row>
-    <row r="39" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-    </row>
-    <row r="40" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-    </row>
-    <row r="41" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-    </row>
-    <row r="42" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-    </row>
-    <row r="43" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-    </row>
-    <row r="44" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-    </row>
-    <row r="45" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-    </row>
-    <row r="46" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-    </row>
-    <row r="47" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-    </row>
-    <row r="48" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-    </row>
-    <row r="49" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-    </row>
-    <row r="50" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-    </row>
-    <row r="51" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-    </row>
-    <row r="52" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-    </row>
-    <row r="53" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-    </row>
-    <row r="54" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-    </row>
-    <row r="55" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-    </row>
-    <row r="56" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-    </row>
-    <row r="57" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-    </row>
-    <row r="58" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-    </row>
-    <row r="59" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-    </row>
-    <row r="60" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-    </row>
-    <row r="61" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-    </row>
-    <row r="62" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="44"/>
+    </row>
+    <row r="22" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+    </row>
+    <row r="23" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+    </row>
+    <row r="24" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+    </row>
+    <row r="25" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+    </row>
+    <row r="26" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+    </row>
+    <row r="28" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+    </row>
+    <row r="29" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+    </row>
+    <row r="31" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+    </row>
+    <row r="32" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+    </row>
+    <row r="33" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+    </row>
+    <row r="34" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+    </row>
+    <row r="35" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+    </row>
+    <row r="36" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+    </row>
+    <row r="37" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+    </row>
+    <row r="38" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+    </row>
+    <row r="39" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+    </row>
+    <row r="40" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+    </row>
+    <row r="41" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+    </row>
+    <row r="42" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+    </row>
+    <row r="43" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+    </row>
+    <row r="44" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+    </row>
+    <row r="45" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+    </row>
+    <row r="46" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+    </row>
+    <row r="47" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+    </row>
+    <row r="48" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+    </row>
+    <row r="49" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+    </row>
+    <row r="50" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+    </row>
+    <row r="51" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+    </row>
+    <row r="52" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+    </row>
+    <row r="53" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+    </row>
+    <row r="54" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+    </row>
+    <row r="55" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+    </row>
+    <row r="56" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+    </row>
+    <row r="57" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+    </row>
+    <row r="58" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+    </row>
+    <row r="59" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+    </row>
+    <row r="60" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+    </row>
+    <row r="61" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+    </row>
+    <row r="62" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C1:X1"/>
+  <mergeCells count="31">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A19:A21"/>
@@ -1488,6 +2012,11 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1495,11 +2024,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM64"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1508,8 +2037,8 @@
     <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
     <col min="3" max="24" width="3.7109375" style="1"/>
     <col min="25" max="27" width="3.7109375" style="5"/>
-    <col min="28" max="28" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="65" width="3.7109375" style="5"/>
+    <col min="28" max="29" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="65" width="3.7109375" style="5"/>
     <col min="66" max="16384" width="3.7109375" style="1"/>
   </cols>
   <sheetData>
@@ -1778,40 +2307,40 @@
       <c r="BM2" s="17"/>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="14">
         <v>1</v>
       </c>
@@ -1880,7 +2409,7 @@
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1910,7 +2439,7 @@
       <c r="X5" s="8"/>
     </row>
     <row r="6" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1938,7 +2467,7 @@
       <c r="X6" s="8"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="9" t="s">
         <v>22</v>
       </c>
@@ -1967,7 +2496,7 @@
       <c r="AB7" s="18"/>
     </row>
     <row r="8" spans="1:65" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1998,7 +2527,7 @@
       <c r="AB8" s="18"/>
     </row>
     <row r="9" spans="1:65" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
@@ -2026,7 +2555,7 @@
       <c r="X9" s="8"/>
     </row>
     <row r="10" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
@@ -2054,7 +2583,7 @@
       <c r="X10" s="8"/>
     </row>
     <row r="11" spans="1:65" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
@@ -2080,9 +2609,16 @@
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
+      <c r="AB11" s="18">
+        <v>45691</v>
+      </c>
+      <c r="AC11" s="18">
+        <f>+AB11+60</f>
+        <v>45751</v>
+      </c>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
@@ -2110,7 +2646,7 @@
       <c r="X12" s="8"/>
     </row>
     <row r="13" spans="1:65" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -2140,7 +2676,7 @@
       <c r="X13" s="8"/>
     </row>
     <row r="14" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
@@ -2168,7 +2704,7 @@
       <c r="X14" s="8"/>
     </row>
     <row r="15" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2196,7 +2732,7 @@
       <c r="X15" s="8"/>
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
@@ -2224,7 +2760,7 @@
       <c r="X16" s="8"/>
     </row>
     <row r="17" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -2254,7 +2790,7 @@
       <c r="X17" s="8"/>
     </row>
     <row r="18" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
@@ -2282,7 +2818,7 @@
       <c r="X18" s="8"/>
     </row>
     <row r="19" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
@@ -2310,7 +2846,7 @@
       <c r="X19" s="8"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
@@ -2338,7 +2874,7 @@
       <c r="X20" s="8"/>
     </row>
     <row r="21" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2368,7 +2904,7 @@
       <c r="X21" s="8"/>
     </row>
     <row r="22" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
@@ -2396,7 +2932,7 @@
       <c r="X22" s="7"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="12" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
jn: referencias bibliograficas y modelo de diccionario de variables
</commit_message>
<xml_diff>
--- a/03_Entregable 1/Cronograma.xlsx
+++ b/03_Entregable 1/Cronograma.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="A entregar" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Producto</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>Semana</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
   </si>
 </sst>
 </file>
@@ -224,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -651,6 +666,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -659,7 +733,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -697,18 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -719,30 +781,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -751,60 +795,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -817,6 +807,78 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -826,6 +888,35 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Estilo 1" xfId="1"/>
@@ -1132,860 +1223,932 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL62"/>
+  <dimension ref="A1:BN62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="23" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="9" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="3.7109375" style="24"/>
-    <col min="24" max="64" width="3.7109375" style="25"/>
-    <col min="65" max="16384" width="3.7109375" style="24"/>
+    <col min="1" max="1" width="15.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="9" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="25" width="3.7109375" style="20"/>
+    <col min="26" max="34" width="3.7109375" style="21"/>
+    <col min="35" max="36" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="37" max="66" width="3.7109375" style="21"/>
+    <col min="67" max="16384" width="3.7109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="71">
+      <c r="D1" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="69"/>
+    </row>
+    <row r="2" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="40">
         <v>1</v>
       </c>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72">
+      <c r="E2" s="41">
         <v>2</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72">
+      <c r="F2" s="41">
         <v>3</v>
       </c>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72">
+      <c r="G2" s="41">
         <v>4</v>
       </c>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72">
+      <c r="H2" s="41">
+        <v>1</v>
+      </c>
+      <c r="I2" s="41">
+        <v>2</v>
+      </c>
+      <c r="J2" s="41">
+        <v>3</v>
+      </c>
+      <c r="K2" s="41">
+        <v>4</v>
+      </c>
+      <c r="L2" s="41">
+        <v>1</v>
+      </c>
+      <c r="M2" s="41">
+        <v>2</v>
+      </c>
+      <c r="N2" s="41">
+        <v>3</v>
+      </c>
+      <c r="O2" s="41">
+        <v>4</v>
+      </c>
+      <c r="P2" s="41">
         <v>5</v>
       </c>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="73"/>
-    </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="68">
+      <c r="Q2" s="41">
         <v>1</v>
       </c>
-      <c r="E2" s="69">
+      <c r="R2" s="41">
         <v>2</v>
       </c>
-      <c r="F2" s="69">
+      <c r="S2" s="41">
         <v>3</v>
       </c>
-      <c r="G2" s="69">
+      <c r="T2" s="41">
         <v>4</v>
       </c>
-      <c r="H2" s="69">
+      <c r="U2" s="41">
+        <v>1</v>
+      </c>
+      <c r="V2" s="41">
+        <v>2</v>
+      </c>
+      <c r="W2" s="41">
+        <v>3</v>
+      </c>
+      <c r="X2" s="77">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="42">
         <v>5</v>
       </c>
-      <c r="I2" s="69">
-        <v>6</v>
-      </c>
-      <c r="J2" s="69">
+    </row>
+    <row r="3" spans="1:36" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="33"/>
+    </row>
+    <row r="4" spans="1:36" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="65"/>
+      <c r="B4" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="54"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="32"/>
+    </row>
+    <row r="5" spans="1:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66"/>
+      <c r="B5" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="80"/>
+      <c r="Y5" s="30"/>
+    </row>
+    <row r="6" spans="1:36" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="78"/>
+      <c r="Y6" s="33"/>
+    </row>
+    <row r="7" spans="1:36" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="62"/>
+      <c r="B7" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="81"/>
+      <c r="Y7" s="31"/>
+    </row>
+    <row r="8" spans="1:36" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62"/>
+      <c r="B8" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="81"/>
+      <c r="Y8" s="31"/>
+    </row>
+    <row r="9" spans="1:36" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="69">
-        <v>8</v>
-      </c>
-      <c r="L2" s="69">
-        <v>9</v>
-      </c>
-      <c r="M2" s="69">
-        <v>10</v>
-      </c>
-      <c r="N2" s="69">
+      <c r="C9" s="48"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="79"/>
+      <c r="Y9" s="32"/>
+      <c r="AI9" s="86"/>
+      <c r="AJ9" s="86"/>
+    </row>
+    <row r="10" spans="1:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="63"/>
+      <c r="B10" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="80"/>
+      <c r="Y10" s="30"/>
+    </row>
+    <row r="11" spans="1:36" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="69">
+      <c r="B11" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="46"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="78"/>
+      <c r="Y11" s="33"/>
+    </row>
+    <row r="12" spans="1:36" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="62"/>
+      <c r="B12" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="56"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="31"/>
+    </row>
+    <row r="13" spans="1:36" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
+      <c r="B13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="69">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="69">
-        <v>14</v>
-      </c>
-      <c r="R2" s="69">
+      <c r="C13" s="48"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="79"/>
+      <c r="Y13" s="32"/>
+    </row>
+    <row r="14" spans="1:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="63"/>
+      <c r="B14" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="44"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="80"/>
+      <c r="Y14" s="30"/>
+    </row>
+    <row r="15" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="69">
+      <c r="B15" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="78"/>
+      <c r="Y15" s="33"/>
+    </row>
+    <row r="16" spans="1:36" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="62"/>
+      <c r="B16" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="83"/>
+      <c r="Y16" s="31"/>
+    </row>
+    <row r="17" spans="1:25" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="62"/>
+      <c r="B17" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="69">
-        <v>17</v>
-      </c>
-      <c r="U2" s="69">
-        <v>18</v>
-      </c>
-      <c r="V2" s="69">
+      <c r="C17" s="54"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="84"/>
+      <c r="Y17" s="32"/>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63"/>
+      <c r="B18" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="85"/>
+      <c r="Y18" s="30"/>
+    </row>
+    <row r="19" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="70">
+      <c r="B19" s="45" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="43"/>
-    </row>
-    <row r="4" spans="1:23" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="42"/>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="1:23" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="43"/>
-    </row>
-    <row r="7" spans="1:23" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="41"/>
-    </row>
-    <row r="8" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
-      <c r="B8" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="41"/>
-    </row>
-    <row r="9" spans="1:23" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="42"/>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="37"/>
-    </row>
-    <row r="11" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="43"/>
-    </row>
-    <row r="12" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
-      <c r="B12" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="41"/>
-    </row>
-    <row r="13" spans="1:23" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="42"/>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="37"/>
-    </row>
-    <row r="15" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="47"/>
-      <c r="R15" s="47"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="47"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="43"/>
-    </row>
-    <row r="16" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="41"/>
-    </row>
-    <row r="17" spans="1:23" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="42"/>
-    </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="37"/>
-    </row>
-    <row r="19" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="33"/>
-      <c r="V19" s="47"/>
-      <c r="W19" s="43"/>
-    </row>
-    <row r="20" spans="1:23" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="59" t="s">
+      <c r="C19" s="46"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="74"/>
+      <c r="X19" s="82"/>
+      <c r="Y19" s="33"/>
+    </row>
+    <row r="20" spans="1:25" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="62"/>
+      <c r="B20" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="48"/>
-    </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="53" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="79"/>
+      <c r="Y20" s="38"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="63"/>
+      <c r="B21" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="44"/>
-    </row>
-    <row r="22" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-    </row>
-    <row r="23" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-    </row>
-    <row r="24" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-    </row>
-    <row r="25" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-    </row>
-    <row r="26" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-    </row>
-    <row r="27" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-    </row>
-    <row r="28" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-    </row>
-    <row r="29" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-    </row>
-    <row r="30" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-    </row>
-    <row r="31" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-    </row>
-    <row r="32" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-    </row>
-    <row r="33" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-    </row>
-    <row r="34" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-    </row>
-    <row r="35" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-    </row>
-    <row r="37" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-    </row>
-    <row r="38" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-    </row>
-    <row r="39" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-    </row>
-    <row r="40" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-    </row>
-    <row r="41" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-    </row>
-    <row r="42" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-    </row>
-    <row r="43" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-    </row>
-    <row r="44" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-    </row>
-    <row r="45" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-    </row>
-    <row r="46" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-    </row>
-    <row r="47" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-    </row>
-    <row r="48" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-    </row>
-    <row r="49" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-    </row>
-    <row r="50" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-    </row>
-    <row r="51" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-    </row>
-    <row r="52" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-    </row>
-    <row r="53" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-    </row>
-    <row r="54" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-    </row>
-    <row r="55" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-    </row>
-    <row r="56" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-    </row>
-    <row r="57" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-    </row>
-    <row r="58" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-    </row>
-    <row r="59" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-    </row>
-    <row r="60" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-    </row>
-    <row r="61" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-    </row>
-    <row r="62" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="80"/>
+      <c r="Y21" s="34"/>
+    </row>
+    <row r="22" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+    </row>
+    <row r="25" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+    </row>
+    <row r="26" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+    </row>
+    <row r="28" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+    </row>
+    <row r="29" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+    </row>
+    <row r="30" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+    </row>
+    <row r="31" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+    </row>
+    <row r="32" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+    </row>
+    <row r="34" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+    </row>
+    <row r="35" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+    </row>
+    <row r="36" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+    </row>
+    <row r="37" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+    </row>
+    <row r="38" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+    </row>
+    <row r="40" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+    </row>
+    <row r="41" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+    </row>
+    <row r="42" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+    </row>
+    <row r="46" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="49" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+    </row>
+    <row r="54" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+    </row>
+    <row r="56" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+    </row>
+    <row r="57" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+    </row>
+    <row r="58" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+    </row>
+    <row r="59" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+    </row>
+    <row r="60" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+    </row>
+    <row r="62" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -1995,28 +2158,6 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2027,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2307,40 +2448,40 @@
       <c r="BM2" s="17"/>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="14">
         <v>1</v>
       </c>
@@ -2409,7 +2550,7 @@
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="70" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2439,7 +2580,7 @@
       <c r="X5" s="8"/>
     </row>
     <row r="6" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -2467,7 +2608,7 @@
       <c r="X6" s="8"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="9" t="s">
         <v>22</v>
       </c>
@@ -2496,7 +2637,7 @@
       <c r="AB7" s="18"/>
     </row>
     <row r="8" spans="1:65" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="70" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2527,7 +2668,7 @@
       <c r="AB8" s="18"/>
     </row>
     <row r="9" spans="1:65" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
@@ -2555,7 +2696,7 @@
       <c r="X9" s="8"/>
     </row>
     <row r="10" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
@@ -2583,7 +2724,7 @@
       <c r="X10" s="8"/>
     </row>
     <row r="11" spans="1:65" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
@@ -2618,7 +2759,7 @@
       </c>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
@@ -2646,7 +2787,7 @@
       <c r="X12" s="8"/>
     </row>
     <row r="13" spans="1:65" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="70" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -2676,7 +2817,7 @@
       <c r="X13" s="8"/>
     </row>
     <row r="14" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
@@ -2704,7 +2845,7 @@
       <c r="X14" s="8"/>
     </row>
     <row r="15" spans="1:65" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2732,7 +2873,7 @@
       <c r="X15" s="8"/>
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
@@ -2760,7 +2901,7 @@
       <c r="X16" s="8"/>
     </row>
     <row r="17" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="70" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -2790,7 +2931,7 @@
       <c r="X17" s="8"/>
     </row>
     <row r="18" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
@@ -2818,7 +2959,7 @@
       <c r="X18" s="8"/>
     </row>
     <row r="19" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
@@ -2846,7 +2987,7 @@
       <c r="X19" s="8"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="9" t="s">
         <v>25</v>
       </c>
@@ -2874,7 +3015,7 @@
       <c r="X20" s="8"/>
     </row>
     <row r="21" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="70" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2904,7 +3045,7 @@
       <c r="X21" s="8"/>
     </row>
     <row r="22" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
@@ -2932,7 +3073,7 @@
       <c r="X22" s="7"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
+      <c r="A23" s="70"/>
       <c r="B23" s="12" t="s">
         <v>26</v>
       </c>

</xml_diff>